<commit_message>
Mudanca do padrao das colunas do XLS padrao para o tipo Texto
</commit_message>
<xml_diff>
--- a/public/downloads/padrao_importacao2.xlsx
+++ b/public/downloads/padrao_importacao2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mansouza\Documents\www\busca-ativa-escolar-lp\public\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A507C885-B17B-49E0-BA8E-6D1F684D59DA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0C95C225-B390-4171-8F3B-9E1BAB0E604D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{CFB3E84B-36E1-41B0-A2CE-7A4B023401E0}"/>
   </bookViews>
@@ -99,12 +99,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,15 +423,16 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="11" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="11" width="15.7109375" style="3" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Mudancas no padrao do arquivo XLS da importacao disponivel para download
</commit_message>
<xml_diff>
--- a/public/downloads/padrao_importacao2.xlsx
+++ b/public/downloads/padrao_importacao2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mansouza\Documents\www\busca-ativa-escolar-lp\public\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0C95C225-B390-4171-8F3B-9E1BAB0E604D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AD3889AD-1AC8-49BF-9F1E-4BE04AF00C96}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{CFB3E84B-36E1-41B0-A2CE-7A4B023401E0}"/>
   </bookViews>
@@ -30,9 +30,6 @@
     <t>Nome do aluno</t>
   </si>
   <si>
-    <t>Data de nascimento</t>
-  </si>
-  <si>
     <t>Nome do pai</t>
   </si>
   <si>
@@ -42,22 +39,25 @@
     <t>Bairro</t>
   </si>
   <si>
-    <t>UF</t>
-  </si>
-  <si>
     <t>Cidade</t>
   </si>
   <si>
-    <t>CEP</t>
-  </si>
-  <si>
-    <t>Telefone</t>
-  </si>
-  <si>
     <t>Observações</t>
   </si>
   <si>
     <t>Nome da mãe ou responsável</t>
+  </si>
+  <si>
+    <t>Data de nascimento: (formato dd/mm/aaaa)</t>
+  </si>
+  <si>
+    <t>UF: (sigla do estado)</t>
+  </si>
+  <si>
+    <t>Telefone: (apenas números com DDD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CEP: (somente números) </t>
   </si>
 </sst>
 </file>
@@ -423,15 +423,21 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="36.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="11" width="15.7109375" style="3" customWidth="1"/>
+    <col min="4" max="5" width="15.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="21" style="3" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="22" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="3" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
@@ -440,34 +446,34 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>